<commit_message>
ZSS-1164: should handle data validation "Cancel" and "Retry" case.
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/1164-cell-switch.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/1164-cell-switch.xlsx
@@ -17,8 +17,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -46,8 +54,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,12 +357,25 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>